<commit_message>
Release V 1.2.1 Ejemplos de Sintesis termnados
</commit_message>
<xml_diff>
--- a/Hard/10-Sintesis_Desde_Excel/Senal Inventada.xlsx
+++ b/Hard/10-Sintesis_Desde_Excel/Senal Inventada.xlsx
@@ -54,9 +54,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -121,7 +120,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.7330927384076991E-2"/>
+          <c:y val="0.13930555555555557"/>
+          <c:w val="0.8680719597550306"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -154,210 +163,222 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$A$1:$A$32</c:f>
+              <c:f>Hoja1!$A$1:$A$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>0.01</c:v>
+                  <c:v>1E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.02</c:v>
+                  <c:v>2.0000000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.03</c:v>
+                  <c:v>2.9999999999999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.04</c:v>
+                  <c:v>4.0000000000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.05</c:v>
+                  <c:v>5.0000000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.06</c:v>
+                  <c:v>5.9999999999999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>6.9999999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.08</c:v>
+                  <c:v>8.0000000000000004E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.09</c:v>
+                  <c:v>8.9999999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1</c:v>
+                  <c:v>1E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.11</c:v>
+                  <c:v>1.1000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.12</c:v>
+                  <c:v>1.1999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.13</c:v>
+                  <c:v>1.2999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>1.4E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.15</c:v>
+                  <c:v>1.5E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.16</c:v>
+                  <c:v>1.6000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.17</c:v>
+                  <c:v>1.6999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.18</c:v>
+                  <c:v>1.8E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.19</c:v>
+                  <c:v>1.9E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.2</c:v>
+                  <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.21</c:v>
+                  <c:v>2.0999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.22</c:v>
+                  <c:v>2.2000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.23</c:v>
+                  <c:v>2.3E-3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.24</c:v>
+                  <c:v>2.3999999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.25</c:v>
+                  <c:v>2.5000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.26</c:v>
+                  <c:v>2.5999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.27</c:v>
+                  <c:v>2.7000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.28000000000000003</c:v>
+                  <c:v>2.8E-3</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.28999999999999998</c:v>
+                  <c:v>2.8999999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.3</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.31</c:v>
+                  <c:v>3.0999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.32</c:v>
+                  <c:v>3.2000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.3E-3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.3999999999999998E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$B$1:$B$32</c:f>
+              <c:f>Hoja1!$B$1:$B$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.1000000000000001</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.2</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.24</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.25</c:v>
-                </c:pt>
-                <c:pt idx="13" formatCode="#,##0">
-                  <c:v>1.256</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.19</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.25</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.24</c:v>
+                  <c:v>0.37</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.2</c:v>
+                  <c:v>0.41</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.1000000000000001</c:v>
+                  <c:v>0.43</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4</c:v>
+                  <c:v>0.43</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4</c:v>
+                  <c:v>0.41</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4</c:v>
+                  <c:v>0.37</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4</c:v>
+                  <c:v>0.19</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4</c:v>
+                  <c:v>2.7</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4</c:v>
+                  <c:v>2.9</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4</c:v>
+                  <c:v>3.03</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4</c:v>
+                  <c:v>3.1</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1</c:v>
+                  <c:v>3.12</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1</c:v>
+                  <c:v>3.1</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1</c:v>
+                  <c:v>3.03</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1</c:v>
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -372,11 +393,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-209494032"/>
-        <c:axId val="-209494576"/>
+        <c:axId val="2034198656"/>
+        <c:axId val="2034192672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-209494032"/>
+        <c:axId val="2034198656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -433,12 +454,12 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-209494576"/>
+        <c:crossAx val="2034192672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-209494576"/>
+        <c:axId val="2034192672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -495,7 +516,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-209494032"/>
+        <c:crossAx val="2034198656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1105,15 +1126,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
+      <xdr:colOff>137266</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:rowOff>164551</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>540026</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>170621</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1398,266 +1419,282 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>0.01</v>
+        <v>1E-4</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.02</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0.03</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0.04</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>0.05</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>0.06</v>
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>7.0000000000000007E-2</v>
+        <v>6.9999999999999999E-4</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>0.08</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>0.09</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
       <c r="B10">
-        <v>1.1000000000000001</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>0.11</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="B11">
-        <v>1.2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>0.12</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="B12">
-        <v>1.24</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>0.13</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="B13">
-        <v>1.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="B14" s="1">
-        <v>1.256</v>
+        <v>1.4E-3</v>
+      </c>
+      <c r="B14">
+        <v>0.19</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>0.15</v>
+        <v>1.5E-3</v>
       </c>
       <c r="B15">
-        <v>1.25</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>0.16</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="B16">
-        <v>1.24</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>0.17</v>
+        <v>1.6999999999999999E-3</v>
       </c>
       <c r="B17">
-        <v>1.2</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>0.18</v>
+        <v>1.8E-3</v>
       </c>
       <c r="B18">
-        <v>1.1000000000000001</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>0.19</v>
+        <v>1.9E-3</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>0.2</v>
+        <v>2E-3</v>
       </c>
       <c r="B20">
-        <v>4</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>0.21</v>
+        <v>2.0999999999999999E-3</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>0.22</v>
+        <v>2.2000000000000001E-3</v>
       </c>
       <c r="B22">
-        <v>4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>0.23</v>
+        <v>2.3E-3</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>0.24</v>
+        <v>2.3999999999999998E-3</v>
       </c>
       <c r="B24">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>0.25</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="B25">
-        <v>4</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>0.26</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="B26">
-        <v>4</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>0.27</v>
+        <v>2.7000000000000001E-3</v>
       </c>
       <c r="B27">
-        <v>4</v>
+        <v>3.03</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>0.28000000000000003</v>
+        <v>2.8E-3</v>
       </c>
       <c r="B28">
-        <v>4</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>0.28999999999999998</v>
+        <v>2.8999999999999998E-3</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>3.12</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>0.3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>0.31</v>
+        <v>3.0999999999999999E-3</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>3.03</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>0.32</v>
+        <v>3.2000000000000002E-3</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>3.3E-3</v>
+      </c>
+      <c r="B33">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>3.3999999999999998E-3</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>